<commit_message>
refactor: Lista conectada ao banco. Implantada uma configuração (não testada) para chamar a API a cada 1s por até 5 vezes caso não haja sucesso devido a API estar dormindo.
</commit_message>
<xml_diff>
--- a/doc/API Noob.xlsx
+++ b/doc/API Noob.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thais\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07fab57a67351b14/0 Fatec/0 Projeto Interdisciplinar/noob/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76272AE-82D2-4D26-B5A0-603279A2F3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{061AA26F-2F7B-4490-A59B-F80A85ADC24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-30" windowWidth="20730" windowHeight="11040" xr2:uid="{F0C2F9E3-B8A7-4FB5-9C76-4CE3FCE4233F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{F0C2F9E3-B8A7-4FB5-9C76-4CE3FCE4233F}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuário" sheetId="1" r:id="rId1"/>
@@ -693,26 +693,26 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{25DA8F6A-B77A-459C-8254-E8D53E88CBAB}" name="Tabela257911" displayName="Tabela257911" ref="G4:J10" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{25DA8F6A-B77A-459C-8254-E8D53E88CBAB}" name="Tabela257911" displayName="Tabela257911" ref="G4:J10" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="G4:J10" xr:uid="{25DA8F6A-B77A-459C-8254-E8D53E88CBAB}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8BABDE45-7E6A-43EF-99BC-F0610D7FE1F0}" name="Funções (controllers)" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{6D6BD8B5-77C9-4CC5-9DA8-A3835D5553AA}" name="Método" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{CB995C1D-F49B-4104-B839-E0BE52725C28}" name="Chamada" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{2CACF18B-B3F7-4CB5-BCA9-C71C59967920}" name="Token" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{8BABDE45-7E6A-43EF-99BC-F0610D7FE1F0}" name="Funções (controllers)" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{6D6BD8B5-77C9-4CC5-9DA8-A3835D5553AA}" name="Método" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{CB995C1D-F49B-4104-B839-E0BE52725C28}" name="Chamada" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{2CACF18B-B3F7-4CB5-BCA9-C71C59967920}" name="Token" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{126C1E3D-B273-491B-9BA2-381505CAD137}" name="Tabela25791113" displayName="Tabela25791113" ref="G4:J10" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{126C1E3D-B273-491B-9BA2-381505CAD137}" name="Tabela25791113" displayName="Tabela25791113" ref="G4:J10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="G4:J10" xr:uid="{126C1E3D-B273-491B-9BA2-381505CAD137}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FCDAE71B-3DC3-45FA-8822-253F91ED670F}" name="Funções (controllers)" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{5D645C2F-95A3-437D-868B-65E95EDCA899}" name="Método" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{4A262960-5D34-4999-B40E-37BDA863F528}" name="Chamada" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{8BF0DFCA-72D4-4531-93E0-1C02190D256C}" name="Token" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{FCDAE71B-3DC3-45FA-8822-253F91ED670F}" name="Funções (controllers)" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{5D645C2F-95A3-437D-868B-65E95EDCA899}" name="Método" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{4A262960-5D34-4999-B40E-37BDA863F528}" name="Chamada" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{8BF0DFCA-72D4-4531-93E0-1C02190D256C}" name="Token" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -816,20 +816,20 @@
     <tableColumn id="1" xr3:uid="{23A61389-4EA6-4A1B-B205-1BC827024EFE}" name="Funções (controllers)" dataDxfId="27"/>
     <tableColumn id="2" xr3:uid="{175D1618-1286-4CC1-A86B-B657A3CDB125}" name="Método" dataDxfId="26"/>
     <tableColumn id="3" xr3:uid="{B14AF4C3-4858-4485-A437-99BAD52AE4F0}" name="Chamada" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{124D8341-09EF-4200-AAE7-EDC43DEE0C24}" name="Token" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{124D8341-09EF-4200-AAE7-EDC43DEE0C24}" name="Token" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D7B5E612-A9AD-457A-8CA6-359B7AB85052}" name="Tabela146810" displayName="Tabela146810" ref="B4:E15" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D7B5E612-A9AD-457A-8CA6-359B7AB85052}" name="Tabela146810" displayName="Tabela146810" ref="B4:E15" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="B4:E15" xr:uid="{D7B5E612-A9AD-457A-8CA6-359B7AB85052}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CE4C0389-F3A7-4304-A964-F75EC482761D}" name="Campos (Model)" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{DCEB81A9-E176-434E-8E12-BA8A67DA0C93}" name="Tipo" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{8A09BE2E-3D2F-4FB8-BE51-8906184A72A1}" name="Obrigatório (required)" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{26235C7A-BA1A-4691-AB95-BECB64A5BEC0}" name="Obs" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{CE4C0389-F3A7-4304-A964-F75EC482761D}" name="Campos (Model)" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{DCEB81A9-E176-434E-8E12-BA8A67DA0C93}" name="Tipo" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{8A09BE2E-3D2F-4FB8-BE51-8906184A72A1}" name="Obrigatório (required)" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{26235C7A-BA1A-4691-AB95-BECB64A5BEC0}" name="Obs" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1154,21 +1154,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E2BC49-5AA6-499A-985C-E7951E3FA866}">
   <dimension ref="B4:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="5" width="22.77734375" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="22.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="70.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.88671875" customWidth="1"/>
+    <col min="9" max="9" width="70.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>90</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>59</v>
       </c>
@@ -1374,21 +1374,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960EE1D2-E140-4CF4-8E3F-B4E26298EB8C}">
   <dimension ref="B4:J17"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="5" width="22.77734375" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="67.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="67.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1550,7 +1550,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1562,7 +1562,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>56</v>
       </c>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>92</v>
       </c>
@@ -1610,7 +1610,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>56</v>
       </c>
@@ -1623,7 +1623,7 @@
       <c r="E16" s="1"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>65</v>
       </c>
@@ -1659,17 +1659,17 @@
       <selection activeCell="J5" sqref="J5:J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="5" width="22.77734375" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="23.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="70.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="70.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>46</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>48</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>57</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>45</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1813,7 +1813,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1823,31 +1823,31 @@
       <c r="I10" s="1"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1877,18 +1877,18 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="22.77734375" customWidth="1"/>
-    <col min="5" max="5" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="2" max="4" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
     <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.36328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>47</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>48</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>100</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>101</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>45</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>102</v>
       </c>
@@ -2050,7 +2050,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>103</v>
       </c>
@@ -2062,7 +2062,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>49</v>
       </c>
@@ -2076,19 +2076,19 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2118,22 +2118,22 @@
       <selection activeCell="B4" sqref="B4:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="22.77734375" customWidth="1"/>
-    <col min="5" max="5" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="72.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.109375" customWidth="1"/>
+    <col min="9" max="9" width="72.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>99</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>55</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>71</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2255,7 +2255,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -2273,7 +2273,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2283,31 +2283,31 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2337,23 +2337,23 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.08984375" customWidth="1"/>
     <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="62.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="95.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="95.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G1" s="3"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>55</v>
       </c>
@@ -2425,7 +2425,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>71</v>
       </c>
@@ -2447,7 +2447,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2461,7 +2461,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -2475,7 +2475,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
@@ -2491,31 +2491,31 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>

</xml_diff>

<commit_message>
instalado o npm install @react-native-async-storage/async-storage
</commit_message>
<xml_diff>
--- a/doc/API Noob.xlsx
+++ b/doc/API Noob.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07fab57a67351b14/0 Fatec/0 Projeto Interdisciplinar/noob/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{D897DEDF-B650-4B15-990D-8809DC29F25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{061AA26F-2F7B-4490-A59B-F80A85ADC24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F0C2F9E3-B8A7-4FB5-9C76-4CE3FCE4233F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{F0C2F9E3-B8A7-4FB5-9C76-4CE3FCE4233F}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuário" sheetId="1" r:id="rId1"/>
@@ -374,10 +374,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -418,21 +425,25 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -669,8 +680,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3717A4B5-940E-406F-9B88-32440B42F2B3}" name="Tabela1" displayName="Tabela1" ref="A1:D8" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
-  <autoFilter ref="A1:D8" xr:uid="{3717A4B5-940E-406F-9B88-32440B42F2B3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3717A4B5-940E-406F-9B88-32440B42F2B3}" name="Tabela1" displayName="Tabela1" ref="B4:E11" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+  <autoFilter ref="B4:E11" xr:uid="{3717A4B5-940E-406F-9B88-32440B42F2B3}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E43BE932-7930-4B3C-9443-FEFACD4F3D2A}" name="Campos (Model)" dataDxfId="69"/>
     <tableColumn id="4" xr3:uid="{B8DD19FB-3218-4296-8ECC-AA0DA5BD27FE}" name="Tipo" dataDxfId="68"/>
@@ -682,8 +693,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{25DA8F6A-B77A-459C-8254-E8D53E88CBAB}" name="Tabela257911" displayName="Tabela257911" ref="F1:I6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="F1:I6" xr:uid="{25DA8F6A-B77A-459C-8254-E8D53E88CBAB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{25DA8F6A-B77A-459C-8254-E8D53E88CBAB}" name="Tabela257911" displayName="Tabela257911" ref="G4:J10" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="G4:J10" xr:uid="{25DA8F6A-B77A-459C-8254-E8D53E88CBAB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8BABDE45-7E6A-43EF-99BC-F0610D7FE1F0}" name="Funções (controllers)" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{6D6BD8B5-77C9-4CC5-9DA8-A3835D5553AA}" name="Método" dataDxfId="14"/>
@@ -695,8 +706,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{126C1E3D-B273-491B-9BA2-381505CAD137}" name="Tabela25791113" displayName="Tabela25791113" ref="F1:I7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="F1:I7" xr:uid="{126C1E3D-B273-491B-9BA2-381505CAD137}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{126C1E3D-B273-491B-9BA2-381505CAD137}" name="Tabela25791113" displayName="Tabela25791113" ref="G4:J10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="G4:J10" xr:uid="{126C1E3D-B273-491B-9BA2-381505CAD137}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{FCDAE71B-3DC3-45FA-8822-253F91ED670F}" name="Funções (controllers)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{5D645C2F-95A3-437D-868B-65E95EDCA899}" name="Método" dataDxfId="8"/>
@@ -708,8 +719,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A4D31A08-1766-437B-AD72-63A1DB6EAD0F}" name="Tabela14681012" displayName="Tabela14681012" ref="A1:D7" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D7" xr:uid="{A4D31A08-1766-437B-AD72-63A1DB6EAD0F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A4D31A08-1766-437B-AD72-63A1DB6EAD0F}" name="Tabela14681012" displayName="Tabela14681012" ref="B4:E15" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="B4:E15" xr:uid="{A4D31A08-1766-437B-AD72-63A1DB6EAD0F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{DEBB1686-5FED-4B11-9F74-FE7820F411CE}" name="Campos (Model)" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{2AB46B0F-334E-40AC-94CF-BD7CFA3B71E2}" name="Tipo" dataDxfId="2"/>
@@ -721,8 +732,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{65A82558-03FE-4CBA-9769-5E0F9DAE01F5}" name="Tabela2" displayName="Tabela2" ref="F1:I7" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
-  <autoFilter ref="F1:I7" xr:uid="{65A82558-03FE-4CBA-9769-5E0F9DAE01F5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{65A82558-03FE-4CBA-9769-5E0F9DAE01F5}" name="Tabela2" displayName="Tabela2" ref="G4:J10" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+  <autoFilter ref="G4:J10" xr:uid="{65A82558-03FE-4CBA-9769-5E0F9DAE01F5}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4EC1EF58-4112-45BF-96AE-5465AD82B0DE}" name="Funções(controllers)" dataDxfId="63"/>
     <tableColumn id="2" xr3:uid="{132A25BF-57B1-4550-8ADB-D93FB7E5665D}" name="Método" dataDxfId="62"/>
@@ -734,8 +745,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C2994A8-ADEB-4DDB-A1D7-B17C1DBC7556}" name="Tabela14" displayName="Tabela14" ref="A1:D14" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
-  <autoFilter ref="A1:D14" xr:uid="{8C2994A8-ADEB-4DDB-A1D7-B17C1DBC7556}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C2994A8-ADEB-4DDB-A1D7-B17C1DBC7556}" name="Tabela14" displayName="Tabela14" ref="B4:E17" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+  <autoFilter ref="B4:E17" xr:uid="{8C2994A8-ADEB-4DDB-A1D7-B17C1DBC7556}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{AA31CE9C-8A5C-47C3-BA69-AA74AF9285BE}" name="Campos (Model)" dataDxfId="57"/>
     <tableColumn id="4" xr3:uid="{5AA5BD48-072F-4A56-9D60-BC3E2DB43F52}" name="Tipo" dataDxfId="56"/>
@@ -747,8 +758,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AB1DE6FB-3815-4E4E-8327-D7EFDDC1635E}" name="Tabela25" displayName="Tabela25" ref="F1:I6" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="F1:I6" xr:uid="{AB1DE6FB-3815-4E4E-8327-D7EFDDC1635E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AB1DE6FB-3815-4E4E-8327-D7EFDDC1635E}" name="Tabela25" displayName="Tabela25" ref="G4:J10" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+  <autoFilter ref="G4:J10" xr:uid="{AB1DE6FB-3815-4E4E-8327-D7EFDDC1635E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9271401C-361E-42EE-94DB-44ACDF38069D}" name="Funções (controllers)" dataDxfId="51"/>
     <tableColumn id="2" xr3:uid="{E2B2D9EC-35E3-4F20-8A1C-B440BBF4E8AF}" name="Método" dataDxfId="50"/>
@@ -760,8 +771,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E795F43B-BAE4-4CE8-8D7E-723B9ADED4D2}" name="Tabela146" displayName="Tabela146" ref="A1:D5" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <autoFilter ref="A1:D5" xr:uid="{E795F43B-BAE4-4CE8-8D7E-723B9ADED4D2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E795F43B-BAE4-4CE8-8D7E-723B9ADED4D2}" name="Tabela146" displayName="Tabela146" ref="B4:E15" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="B4:E15" xr:uid="{E795F43B-BAE4-4CE8-8D7E-723B9ADED4D2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C7695CEC-A311-4630-8A0F-B0C184743BEC}" name="Campos (Model)" dataDxfId="45"/>
     <tableColumn id="4" xr3:uid="{0050FA34-F962-401B-913A-F996C0FDC143}" name="Tipo" dataDxfId="44"/>
@@ -773,8 +784,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5B258DBD-4CC1-44C3-8308-0462D9859036}" name="Tabela257" displayName="Tabela257" ref="F1:I6" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="F1:I6" xr:uid="{5B258DBD-4CC1-44C3-8308-0462D9859036}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5B258DBD-4CC1-44C3-8308-0462D9859036}" name="Tabela257" displayName="Tabela257" ref="G4:J10" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="G4:J10" xr:uid="{5B258DBD-4CC1-44C3-8308-0462D9859036}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7705D4D3-E8DE-43F5-8AA7-07101EC3E72D}" name="Funções (controllers)" dataDxfId="39"/>
     <tableColumn id="2" xr3:uid="{1E5D0C9D-F2DE-4002-8714-64C70791F566}" name="Método" dataDxfId="38"/>
@@ -786,8 +797,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DCDECD88-F26D-4371-B8AB-7B26706E540C}" name="Tabela1468" displayName="Tabela1468" ref="A1:D9" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:D9" xr:uid="{DCDECD88-F26D-4371-B8AB-7B26706E540C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DCDECD88-F26D-4371-B8AB-7B26706E540C}" name="Tabela1468" displayName="Tabela1468" ref="B4:E15" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="B4:E15" xr:uid="{DCDECD88-F26D-4371-B8AB-7B26706E540C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{478527A8-C817-46BA-BC43-41A177B91883}" name="Campos (Model)" dataDxfId="33"/>
     <tableColumn id="4" xr3:uid="{86DC36D0-0104-4A43-9D12-3084FE9F464E}" name="Tipo" dataDxfId="32"/>
@@ -799,8 +810,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{95651ABC-A381-4308-AA7C-837F47BE4482}" name="Tabela2579" displayName="Tabela2579" ref="F1:I6" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="F1:I6" xr:uid="{95651ABC-A381-4308-AA7C-837F47BE4482}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{95651ABC-A381-4308-AA7C-837F47BE4482}" name="Tabela2579" displayName="Tabela2579" ref="G4:J10" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="G4:J10" xr:uid="{95651ABC-A381-4308-AA7C-837F47BE4482}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{23A61389-4EA6-4A1B-B205-1BC827024EFE}" name="Funções (controllers)" dataDxfId="27"/>
     <tableColumn id="2" xr3:uid="{175D1618-1286-4CC1-A86B-B657A3CDB125}" name="Método" dataDxfId="26"/>
@@ -812,8 +823,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D7B5E612-A9AD-457A-8CA6-359B7AB85052}" name="Tabela146810" displayName="Tabela146810" ref="A1:D4" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:D4" xr:uid="{D7B5E612-A9AD-457A-8CA6-359B7AB85052}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D7B5E612-A9AD-457A-8CA6-359B7AB85052}" name="Tabela146810" displayName="Tabela146810" ref="B4:E15" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B4:E15" xr:uid="{D7B5E612-A9AD-457A-8CA6-359B7AB85052}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{CE4C0389-F3A7-4304-A964-F75EC482761D}" name="Campos (Model)" dataDxfId="21"/>
     <tableColumn id="4" xr3:uid="{DCEB81A9-E176-434E-8E12-BA8A67DA0C93}" name="Tipo" dataDxfId="20"/>
@@ -1141,215 +1152,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E2BC49-5AA6-499A-985C-E7951E3FA866}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="B4:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="22.81640625" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
-    <col min="6" max="6" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="70.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.90625" customWidth="1"/>
+    <col min="2" max="5" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="70.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="E5" s="1"/>
+      <c r="G5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="E6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="F4" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="F5" s="1" t="s">
+      <c r="E8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="F6" s="1" t="s">
+      <c r="E9" s="1"/>
+      <c r="G9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I10" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="I8" s="5"/>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="J11" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{1459769A-C565-4DD2-B42A-1F8ACB900822}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{FE8E8170-1C6D-4B55-99F3-23D97F7AC092}"/>
-    <hyperlink ref="H2" r:id="rId3" xr:uid="{C3CD15BF-E056-47EC-8683-DFCBE24E1A06}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{650A7906-593B-47A6-9653-0852A8F6C26E}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{61F5279E-B082-474F-92CA-AD856BCCB5F2}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{7B38C964-E59D-413D-883B-60B62E99A686}"/>
+    <hyperlink ref="I6" r:id="rId1" xr:uid="{1459769A-C565-4DD2-B42A-1F8ACB900822}"/>
+    <hyperlink ref="I7" r:id="rId2" xr:uid="{FE8E8170-1C6D-4B55-99F3-23D97F7AC092}"/>
+    <hyperlink ref="I5" r:id="rId3" xr:uid="{C3CD15BF-E056-47EC-8683-DFCBE24E1A06}"/>
+    <hyperlink ref="I8" r:id="rId4" xr:uid="{650A7906-593B-47A6-9653-0852A8F6C26E}"/>
+    <hyperlink ref="I9" r:id="rId5" xr:uid="{61F5279E-B082-474F-92CA-AD856BCCB5F2}"/>
+    <hyperlink ref="I10" r:id="rId6" xr:uid="{7B38C964-E59D-413D-883B-60B62E99A686}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="2">
@@ -1361,276 +1372,276 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960EE1D2-E140-4CF4-8E3F-B4E26298EB8C}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="B4:J17"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="22.81640625" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
-    <col min="6" max="6" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.36328125" customWidth="1"/>
+    <col min="2" max="5" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="67.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="E5" s="1"/>
+      <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="F4" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="F5" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I8" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="F6" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{76A24ACB-DA98-4ED2-B2F9-ABEB9C3FD524}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{2F4ABC68-FCFB-4185-B947-5C1C2169010C}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{A11F5257-1D0A-47AA-BFA5-5C3F2731FB6D}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{4F903700-1026-4933-9805-F415DA89793E}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{6BF1DF5D-8A2D-4B67-B85F-139237BE0132}"/>
+    <hyperlink ref="I5" r:id="rId1" xr:uid="{76A24ACB-DA98-4ED2-B2F9-ABEB9C3FD524}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{2F4ABC68-FCFB-4185-B947-5C1C2169010C}"/>
+    <hyperlink ref="I7" r:id="rId3" xr:uid="{A11F5257-1D0A-47AA-BFA5-5C3F2731FB6D}"/>
+    <hyperlink ref="I8" r:id="rId4" xr:uid="{4F903700-1026-4933-9805-F415DA89793E}"/>
+    <hyperlink ref="I9" r:id="rId5" xr:uid="{6BF1DF5D-8A2D-4B67-B85F-139237BE0132}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="2">
@@ -1642,213 +1653,213 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E636A4-74F4-4B12-8705-A6D1B445F3FE}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="B4:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="J5" sqref="J5:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="22.81640625" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
-    <col min="6" max="6" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="70.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.36328125" customWidth="1"/>
+    <col min="2" max="5" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="70.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I6" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I7" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="F5" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I8" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{3FDC3FD8-7745-4326-A71A-A09EAACD5AA9}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{33866C6E-1BE5-4660-8CE4-803123C6C4D8}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{C6B122EA-C95C-4A26-BAE9-530AED833FF9}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{93FB5CAC-910A-418C-824B-CEE504B36A5E}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{B6C298FC-1278-4AB9-AB6D-0BC698EE6C3E}"/>
+    <hyperlink ref="I5" r:id="rId1" xr:uid="{3FDC3FD8-7745-4326-A71A-A09EAACD5AA9}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{33866C6E-1BE5-4660-8CE4-803123C6C4D8}"/>
+    <hyperlink ref="I7" r:id="rId3" xr:uid="{C6B122EA-C95C-4A26-BAE9-530AED833FF9}"/>
+    <hyperlink ref="I8" r:id="rId4" xr:uid="{93FB5CAC-910A-418C-824B-CEE504B36A5E}"/>
+    <hyperlink ref="I9" r:id="rId5" xr:uid="{B6C298FC-1278-4AB9-AB6D-0BC698EE6C3E}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="2">
@@ -1860,236 +1871,236 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554CB4A8-BD70-4A13-846E-7C1892696148}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="B4:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
-    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="72.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27" customWidth="1"/>
+    <col min="2" max="4" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="G5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="F4" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I7" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="F5" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="F6" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="G9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I9" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{8C0C3B03-1AE7-4080-913F-88C9C0156B30}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{FFBD8CB7-7724-40EA-B797-A35258DFA142}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{D23BDBB9-E791-4837-AAC1-951A7E8C4ED9}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{69005D7B-F11D-48B6-80B4-65A13F754437}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{4857F2D9-3BD8-4F64-A5BC-76F54474C7E4}"/>
+    <hyperlink ref="I5" r:id="rId1" xr:uid="{8C0C3B03-1AE7-4080-913F-88C9C0156B30}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{FFBD8CB7-7724-40EA-B797-A35258DFA142}"/>
+    <hyperlink ref="I7" r:id="rId3" xr:uid="{D23BDBB9-E791-4837-AAC1-951A7E8C4ED9}"/>
+    <hyperlink ref="I8" r:id="rId4" xr:uid="{69005D7B-F11D-48B6-80B4-65A13F754437}"/>
+    <hyperlink ref="I9" r:id="rId5" xr:uid="{4857F2D9-3BD8-4F64-A5BC-76F54474C7E4}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="2">
@@ -2101,210 +2112,214 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C1C4EF-97BF-4034-8CE4-BAFFD73C21AB}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="B1:J15"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B4" sqref="B4:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="30.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
-    <col min="6" max="6" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="72.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.08984375" customWidth="1"/>
+    <col min="2" max="4" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="72.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H5" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I5" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I6" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I7" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{36623095-5756-4B61-BF1A-423CFB79E706}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{1D9C9740-A210-4572-AAFB-B67309A7BC5E}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{98A2A006-EDA0-482D-932B-98FD147903B8}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{72FBDD99-2B87-4DDD-9FC6-8484234709ED}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{599F515F-3EF8-43DA-A978-41697D66092C}"/>
+    <hyperlink ref="I5" r:id="rId1" xr:uid="{36623095-5756-4B61-BF1A-423CFB79E706}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{1D9C9740-A210-4572-AAFB-B67309A7BC5E}"/>
+    <hyperlink ref="I7" r:id="rId3" xr:uid="{98A2A006-EDA0-482D-932B-98FD147903B8}"/>
+    <hyperlink ref="I8" r:id="rId4" xr:uid="{72FBDD99-2B87-4DDD-9FC6-8484234709ED}"/>
+    <hyperlink ref="I9" r:id="rId5" xr:uid="{599F515F-3EF8-43DA-A978-41697D66092C}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="2">
@@ -2316,196 +2331,199 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01FAF138-4431-4EF9-BE2C-326788863ACC}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="B1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" customWidth="1"/>
-    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="95.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.08984375" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="95.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="G1" s="3"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="E5" s="1"/>
+      <c r="G5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="2:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{C75ED29F-470E-4D41-AE01-F9895A66AD30}"/>
+    <hyperlink ref="I5" r:id="rId1" xr:uid="{C75ED29F-470E-4D41-AE01-F9895A66AD30}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="2">

</xml_diff>